<commit_message>
run the static simulation
</commit_message>
<xml_diff>
--- a/fault-level-01.xlsx
+++ b/fault-level-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afiq Hafizuddin\Documents\MATLAB\01-STATIC-DUMA-AMEND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE008AF-5F18-41B2-A100-D09986FE647E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5102BBF9-C0D5-434B-ACEA-AF7F7AAFDC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parallel" sheetId="1" r:id="rId1"/>
@@ -189,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,6 +232,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,7 +847,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection sqref="A1:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,14 +981,14 @@
       <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="4">
-        <v>16826</v>
+      <c r="E5" s="15">
+        <v>12391</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="4">
-        <v>16849</v>
+      <c r="G5" s="15">
+        <v>12411</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>6</v>
@@ -996,12 +999,12 @@
       <c r="J5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="4">
-        <v>16907</v>
+      <c r="K5" s="15">
+        <v>12461</v>
       </c>
       <c r="L5" s="4"/>
-      <c r="M5" s="4">
-        <v>16907</v>
+      <c r="M5" s="15">
+        <v>12461</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>6</v>
@@ -1014,47 +1017,47 @@
       <c r="B6" s="4">
         <v>20</v>
       </c>
-      <c r="C6" s="4">
-        <v>22526</v>
+      <c r="C6" s="15">
+        <v>22528</v>
       </c>
       <c r="D6" s="4">
         <f>(C6-C$5)</f>
-        <v>26</v>
-      </c>
-      <c r="E6" s="4">
-        <v>16845</v>
+        <v>28</v>
+      </c>
+      <c r="E6" s="15">
+        <v>12405</v>
       </c>
       <c r="F6" s="4">
         <f>(E6-E$5)</f>
-        <v>19</v>
-      </c>
-      <c r="G6" s="4">
-        <v>16871</v>
+        <v>14</v>
+      </c>
+      <c r="G6" s="15">
+        <v>12428</v>
       </c>
       <c r="H6" s="4">
         <f>(G6-G$5)</f>
-        <v>22</v>
-      </c>
-      <c r="I6" s="4">
-        <v>22524</v>
+        <v>17</v>
+      </c>
+      <c r="I6" s="15">
+        <v>22525</v>
       </c>
       <c r="J6" s="4">
         <f>(I6-I$5)</f>
-        <v>24</v>
-      </c>
-      <c r="K6" s="4">
-        <v>16926</v>
+        <v>25</v>
+      </c>
+      <c r="K6" s="15">
+        <v>12475</v>
       </c>
       <c r="L6" s="4">
         <f>(K6-K$5)</f>
-        <v>19</v>
-      </c>
-      <c r="M6" s="4">
-        <v>16930</v>
+        <v>14</v>
+      </c>
+      <c r="M6" s="15">
+        <v>12479</v>
       </c>
       <c r="N6" s="4">
         <f>(M6-M$5)</f>
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -1064,47 +1067,47 @@
       <c r="B7" s="4">
         <v>40</v>
       </c>
-      <c r="C7" s="4">
-        <v>22553</v>
+      <c r="C7" s="15">
+        <v>22558</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" ref="D7:D10" si="0">(C7-C$5)</f>
-        <v>53</v>
-      </c>
-      <c r="E7" s="4">
-        <v>16865</v>
+        <v>58</v>
+      </c>
+      <c r="E7" s="15">
+        <v>12421</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" ref="F7:F10" si="1">(E7-E$5)</f>
-        <v>39</v>
-      </c>
-      <c r="G7" s="4">
-        <v>16897</v>
+        <v>30</v>
+      </c>
+      <c r="G7" s="15">
+        <v>12449</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" ref="H7:H10" si="2">(G7-G$5)</f>
-        <v>48</v>
-      </c>
-      <c r="I7" s="4">
-        <v>22550</v>
+        <v>38</v>
+      </c>
+      <c r="I7" s="15">
+        <v>22552</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" ref="J7:J10" si="3">(I7-I$5)</f>
-        <v>50</v>
-      </c>
-      <c r="K7" s="4">
-        <v>16947</v>
+        <v>52</v>
+      </c>
+      <c r="K7" s="15">
+        <v>12492</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" ref="L7:L10" si="4">(K7-K$5)</f>
-        <v>40</v>
-      </c>
-      <c r="M7" s="4">
-        <v>16956</v>
+        <v>31</v>
+      </c>
+      <c r="M7" s="15">
+        <v>12500</v>
       </c>
       <c r="N7" s="4">
         <f t="shared" ref="N7:N10" si="5">(M7-M$5)</f>
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1114,47 +1117,47 @@
       <c r="B8" s="4">
         <v>60</v>
       </c>
-      <c r="C8" s="4">
-        <v>22582</v>
+      <c r="C8" s="15">
+        <v>22589</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>82</v>
-      </c>
-      <c r="E8" s="4">
-        <v>16886</v>
+        <v>89</v>
+      </c>
+      <c r="E8" s="15">
+        <v>12438</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="G8" s="4">
-        <v>16924</v>
+        <v>47</v>
+      </c>
+      <c r="G8" s="15">
+        <v>12473</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="2"/>
-        <v>75</v>
-      </c>
-      <c r="I8" s="4">
-        <v>22577</v>
+        <v>62</v>
+      </c>
+      <c r="I8" s="15">
+        <v>22581</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="3"/>
-        <v>77</v>
-      </c>
-      <c r="K8" s="4">
-        <v>16969</v>
+        <v>81</v>
+      </c>
+      <c r="K8" s="15">
+        <v>12510</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="4"/>
-        <v>62</v>
-      </c>
-      <c r="M8" s="4">
-        <v>16985</v>
+        <v>49</v>
+      </c>
+      <c r="M8" s="15">
+        <v>12525</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" si="5"/>
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1164,47 +1167,47 @@
       <c r="B9" s="4">
         <v>80</v>
       </c>
-      <c r="C9" s="4">
-        <v>22611</v>
+      <c r="C9" s="15">
+        <v>22622</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>111</v>
-      </c>
-      <c r="E9" s="4">
-        <v>16909</v>
+        <v>122</v>
+      </c>
+      <c r="E9" s="15">
+        <v>12457</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="G9" s="4">
-        <v>16954</v>
+        <v>66</v>
+      </c>
+      <c r="G9" s="15">
+        <v>12499</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="I9" s="4">
-        <v>22605</v>
+        <v>88</v>
+      </c>
+      <c r="I9" s="15">
+        <v>22612</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="3"/>
-        <v>105</v>
-      </c>
-      <c r="K9" s="4">
-        <v>16993</v>
+        <v>112</v>
+      </c>
+      <c r="K9" s="15">
+        <v>12530</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="4"/>
-        <v>86</v>
-      </c>
-      <c r="M9" s="4">
-        <v>17015</v>
+        <v>69</v>
+      </c>
+      <c r="M9" s="15">
+        <v>12552</v>
       </c>
       <c r="N9" s="4">
         <f t="shared" si="5"/>
-        <v>108</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1214,47 +1217,47 @@
       <c r="B10" s="4">
         <v>100</v>
       </c>
-      <c r="C10" s="4">
-        <v>22642</v>
+      <c r="C10" s="15">
+        <v>22657</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>142</v>
-      </c>
-      <c r="E10" s="4">
-        <v>16933</v>
+        <v>157</v>
+      </c>
+      <c r="E10" s="15">
+        <v>12478</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="1"/>
-        <v>107</v>
-      </c>
-      <c r="G10" s="4">
-        <v>16987</v>
+        <v>87</v>
+      </c>
+      <c r="G10" s="15">
+        <v>12529</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="2"/>
-        <v>138</v>
-      </c>
-      <c r="I10" s="4">
-        <v>22634</v>
+        <v>118</v>
+      </c>
+      <c r="I10" s="15">
+        <v>22644</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="3"/>
-        <v>134</v>
-      </c>
-      <c r="K10" s="4">
-        <v>17018</v>
+        <v>144</v>
+      </c>
+      <c r="K10" s="15">
+        <v>12551</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="4"/>
-        <v>111</v>
-      </c>
-      <c r="M10" s="4">
-        <v>17049</v>
+        <v>90</v>
+      </c>
+      <c r="M10" s="15">
+        <v>12583</v>
       </c>
       <c r="N10" s="4">
         <f t="shared" si="5"/>
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1287,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F660670-0344-40C3-B538-6C422568AB92}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1372,14 +1375,14 @@
       <c r="B4" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>22500</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="4">
-        <v>12647</v>
+        <v>12461</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>6</v>
@@ -1391,7 +1394,7 @@
         <v>6</v>
       </c>
       <c r="I4" s="4">
-        <v>12647</v>
+        <v>12461</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>6</v>
@@ -1405,28 +1408,28 @@
         <v>20</v>
       </c>
       <c r="C5" s="4">
-        <v>22530</v>
+        <v>22531</v>
       </c>
       <c r="D5" s="5">
         <f>(C5-C$4)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" s="4">
-        <v>12673</v>
+        <v>12488</v>
       </c>
       <c r="F5" s="4">
         <f>(E5-E$4)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" s="4">
-        <v>22525</v>
+        <v>22526</v>
       </c>
       <c r="H5" s="4">
         <f>(G5-G$4)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I5" s="4">
-        <v>12673</v>
+        <v>12487</v>
       </c>
       <c r="J5" s="4">
         <f>(I5-I$4)</f>
@@ -1441,32 +1444,32 @@
         <v>40</v>
       </c>
       <c r="C6" s="4">
-        <v>22562</v>
+        <v>22564</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" ref="D6:D9" si="0">(C6-C$4)</f>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E6" s="4">
-        <v>12707</v>
+        <v>12522</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" ref="F6:F9" si="1">(E6-E$4)</f>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G6" s="4">
-        <v>22553</v>
+        <v>22555</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" ref="H6:H9" si="2">(G6-G$4)</f>
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I6" s="4">
-        <v>12706</v>
+        <v>12521</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" ref="J6:J9" si="3">(I6-I$4)</f>
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1477,32 +1480,32 @@
         <v>60</v>
       </c>
       <c r="C7" s="4">
-        <v>22596</v>
+        <v>22600</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E7" s="4">
-        <v>12747</v>
+        <v>12563</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G7" s="4">
-        <v>22583</v>
+        <v>22587</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="2"/>
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="I7" s="4">
-        <v>12746</v>
+        <v>12562</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="3"/>
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1513,32 +1516,32 @@
         <v>80</v>
       </c>
       <c r="C8" s="4">
-        <v>22632</v>
+        <v>22639</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="E8" s="4">
-        <v>12794</v>
+        <v>12611</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G8" s="4">
-        <v>22616</v>
+        <v>22621</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="2"/>
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="I8" s="4">
-        <v>12793</v>
+        <v>12611</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="3"/>
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1549,32 +1552,32 @@
         <v>100</v>
       </c>
       <c r="C9" s="4">
-        <v>22671</v>
+        <v>22679</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="0"/>
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E9" s="4">
-        <v>12847</v>
+        <v>12666</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="G9" s="4">
-        <v>22652</v>
+        <v>22659</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="I9" s="4">
-        <v>12847</v>
+        <v>12666</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1592,5 +1595,6 @@
     <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>